<commit_message>
adding media to ep04
</commit_message>
<xml_diff>
--- a/media/Metrics.xlsx
+++ b/media/Metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BlazQ\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CF52E4-E9B6-47E9-B4B7-607DAF85ED3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14213EC9-4342-4BF2-90CE-23BFB6A3852B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{B5ACBA44-7870-4F88-9599-E80736D0BCDD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B5ACBA44-7870-4F88-9599-E80736D0BCDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Episode</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Total Views</t>
+  </si>
+  <si>
+    <t>EP03</t>
   </si>
 </sst>
 </file>
@@ -272,15 +275,18 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$3</c:f>
+              <c:f>Data!$G$2:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -588,15 +594,18 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$3</c:f>
+              <c:f>Data!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -694,15 +703,18 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$3</c:f>
+              <c:f>Data!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -800,14 +812,17 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$D$2:$D$3</c:f>
+              <c:f>Data!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -906,14 +921,17 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$E$2:$E$3</c:f>
+              <c:f>Data!$E$2:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1012,15 +1030,18 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$F$2:$F$3</c:f>
+              <c:f>Data!$F$2:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1401,29 +1422,35 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$3</c:f>
+              <c:f>Data!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>EP 01</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>EP 02</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>EP03</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$3</c:f>
+              <c:f>Data!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1527,29 +1554,35 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$3</c:f>
+              <c:f>Data!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>EP 01</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>EP 02</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>EP03</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$3</c:f>
+              <c:f>Data!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3595,7 +3628,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B84BBFF9-22ED-4F2D-AE5E-E0D34D554333}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3606,7 +3639,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{4CA1CA02-9723-4562-9600-7016A7B868A4}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3617,7 +3650,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{7F779538-D910-408C-ABD9-2E25E6814FCF}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3661,7 +3694,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8654815" cy="6274741"/>
+    <xdr:ext cx="8656674" cy="6282070"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3694,7 +3727,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8654815" cy="6274741"/>
+    <xdr:ext cx="8656674" cy="6282070"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3724,8 +3757,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B907DECD-DC64-4049-B0C9-13B7A2500D59}" name="Table1" displayName="Table1" ref="A1:G3" totalsRowShown="0">
-  <autoFilter ref="A1:G3" xr:uid="{FDB90191-74AE-42DF-A1FC-4B9073DE7BAA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B907DECD-DC64-4049-B0C9-13B7A2500D59}" name="Table1" displayName="Table1" ref="A1:G4" totalsRowShown="0">
+  <autoFilter ref="A1:G4" xr:uid="{FDB90191-74AE-42DF-A1FC-4B9073DE7BAA}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{DB21C1C3-9D22-4282-A7B6-91CE6962695D}" name="Episode"/>
     <tableColumn id="2" xr3:uid="{2F72E6BD-6B24-41C9-A2DB-EC622920686E}" name="Live"/>
@@ -4036,10 +4069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D00B6F-E49B-4CB0-8510-4C0095FEF97A}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4118,6 +4151,29 @@
         <v>87</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
ep05 after show work
</commit_message>
<xml_diff>
--- a/media/Metrics.xlsx
+++ b/media/Metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BlazQ\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14213EC9-4342-4BF2-90CE-23BFB6A3852B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9476D9-6948-4B8B-A192-1BCDACD29E71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B5ACBA44-7870-4F88-9599-E80736D0BCDD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B5ACBA44-7870-4F88-9599-E80736D0BCDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Episode</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>EP03</t>
+  </si>
+  <si>
+    <t>EP04</t>
   </si>
 </sst>
 </file>
@@ -275,10 +278,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$4</c:f>
+              <c:f>Data!$G$2:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>33</c:v>
                 </c:pt>
@@ -287,6 +290,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -594,10 +600,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$4</c:f>
+              <c:f>Data!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -606,6 +612,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -703,10 +712,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$4</c:f>
+              <c:f>Data!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>24</c:v>
                 </c:pt>
@@ -715,6 +724,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -812,10 +824,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$D$2:$D$4</c:f>
+              <c:f>Data!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -823,6 +835,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -921,10 +936,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$E$2:$E$4</c:f>
+              <c:f>Data!$E$2:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -932,6 +947,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1030,10 +1048,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$F$2:$F$4</c:f>
+              <c:f>Data!$F$2:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -1041,6 +1059,9 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1422,9 +1443,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$4</c:f>
+              <c:f>Data!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>EP 01</c:v>
                 </c:pt>
@@ -1433,16 +1454,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>EP03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EP04</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$4</c:f>
+              <c:f>Data!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1451,6 +1475,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1554,9 +1581,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$4</c:f>
+              <c:f>Data!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>EP 01</c:v>
                 </c:pt>
@@ -1565,16 +1592,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>EP03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EP04</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$4</c:f>
+              <c:f>Data!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>24</c:v>
                 </c:pt>
@@ -1583,6 +1613,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3628,7 +3661,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B84BBFF9-22ED-4F2D-AE5E-E0D34D554333}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3661,7 +3694,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8645769" cy="6271846"/>
+    <xdr:ext cx="8656674" cy="6282070"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3757,8 +3790,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B907DECD-DC64-4049-B0C9-13B7A2500D59}" name="Table1" displayName="Table1" ref="A1:G4" totalsRowShown="0">
-  <autoFilter ref="A1:G4" xr:uid="{FDB90191-74AE-42DF-A1FC-4B9073DE7BAA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B907DECD-DC64-4049-B0C9-13B7A2500D59}" name="Table1" displayName="Table1" ref="A1:G5" totalsRowShown="0">
+  <autoFilter ref="A1:G5" xr:uid="{FDB90191-74AE-42DF-A1FC-4B9073DE7BAA}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{DB21C1C3-9D22-4282-A7B6-91CE6962695D}" name="Episode"/>
     <tableColumn id="2" xr3:uid="{2F72E6BD-6B24-41C9-A2DB-EC622920686E}" name="Live"/>
@@ -4069,10 +4102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D00B6F-E49B-4CB0-8510-4C0095FEF97A}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4174,6 +4207,29 @@
         <v>98</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
update metric for ep06
</commit_message>
<xml_diff>
--- a/media/Metrics.xlsx
+++ b/media/Metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BlazQ\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9476D9-6948-4B8B-A192-1BCDACD29E71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796F44E5-4336-419A-8935-637C46C31C14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B5ACBA44-7870-4F88-9599-E80736D0BCDD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B5ACBA44-7870-4F88-9599-E80736D0BCDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Episode</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>EP04</t>
+  </si>
+  <si>
+    <t>EP05</t>
   </si>
 </sst>
 </file>
@@ -278,10 +281,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$2:$G$5</c:f>
+              <c:f>Data!$G$2:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>33</c:v>
                 </c:pt>
@@ -293,6 +296,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -600,10 +606,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$5</c:f>
+              <c:f>Data!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -615,6 +621,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -712,10 +721,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$5</c:f>
+              <c:f>Data!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>24</c:v>
                 </c:pt>
@@ -727,6 +736,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -824,10 +836,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$D$2:$D$5</c:f>
+              <c:f>Data!$D$2:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -838,6 +850,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -936,10 +951,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$E$2:$E$5</c:f>
+              <c:f>Data!$E$2:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -950,6 +965,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1048,10 +1066,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Data!$F$2:$F$5</c:f>
+              <c:f>Data!$F$2:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -1062,6 +1080,9 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1443,9 +1464,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$5</c:f>
+              <c:f>Data!$A$2:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>EP 01</c:v>
                 </c:pt>
@@ -1457,16 +1478,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>EP04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>EP05</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$5</c:f>
+              <c:f>Data!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1478,6 +1502,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1581,9 +1608,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$5</c:f>
+              <c:f>Data!$A$2:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>EP 01</c:v>
                 </c:pt>
@@ -1595,16 +1622,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>EP04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>EP05</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$5</c:f>
+              <c:f>Data!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>24</c:v>
                 </c:pt>
@@ -1616,6 +1646,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3672,7 +3705,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{4CA1CA02-9723-4562-9600-7016A7B868A4}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3790,8 +3823,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B907DECD-DC64-4049-B0C9-13B7A2500D59}" name="Table1" displayName="Table1" ref="A1:G5" totalsRowShown="0">
-  <autoFilter ref="A1:G5" xr:uid="{FDB90191-74AE-42DF-A1FC-4B9073DE7BAA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B907DECD-DC64-4049-B0C9-13B7A2500D59}" name="Table1" displayName="Table1" ref="A1:G6" totalsRowShown="0">
+  <autoFilter ref="A1:G6" xr:uid="{FDB90191-74AE-42DF-A1FC-4B9073DE7BAA}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{DB21C1C3-9D22-4282-A7B6-91CE6962695D}" name="Episode"/>
     <tableColumn id="2" xr3:uid="{2F72E6BD-6B24-41C9-A2DB-EC622920686E}" name="Live"/>
@@ -4102,10 +4135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D00B6F-E49B-4CB0-8510-4C0095FEF97A}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4230,6 +4263,29 @@
         <v>114</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>